<commit_message>
Katmanlı Mimari Olusturuldu -group
</commit_message>
<xml_diff>
--- a/ProjePlanı.xlsx
+++ b/ProjePlanı.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{072BAEAE-82AA-4C7C-811D-4EFCB640C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B8C671-C4EB-4806-97FD-B3715FB0BD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="855" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
-    <sheet name="About" sheetId="12" r:id="rId2"/>
+    <sheet name="Sayfa1" sheetId="13" r:id="rId2"/>
+    <sheet name="About" sheetId="12" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Display_Week">ProjectSchedule!$E$4</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="108">
   <si>
     <t>Task 3</t>
   </si>
@@ -290,6 +291,120 @@
   </si>
   <si>
     <t>Form2  Kayıt Olma Arayüz (Ad,Soyad,KullanıcıAdı,ProfilResmi,Mail, Şifrre, Şifre Tekrar, Cinsiyet,Boy,Kilo)</t>
+  </si>
+  <si>
+    <t>Tablolar</t>
+  </si>
+  <si>
+    <t>Kullanıcılar</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Ad</t>
+  </si>
+  <si>
+    <t>Soyad</t>
+  </si>
+  <si>
+    <t>Kullanıcı Adi</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>Şifre</t>
+  </si>
+  <si>
+    <t>Boy</t>
+  </si>
+  <si>
+    <t>Kilo</t>
+  </si>
+  <si>
+    <t>Cinsiyet</t>
+  </si>
+  <si>
+    <t>Fotoğraf</t>
+  </si>
+  <si>
+    <t>(Enum)</t>
+  </si>
+  <si>
+    <t>Öğün</t>
+  </si>
+  <si>
+    <t>ÖğünID</t>
+  </si>
+  <si>
+    <t>Öğün Adı</t>
+  </si>
+  <si>
+    <t>Kategori</t>
+  </si>
+  <si>
+    <t>KatID</t>
+  </si>
+  <si>
+    <t>Kalori</t>
+  </si>
+  <si>
+    <t>(adet,yemek kaşığı,kase,litre)</t>
+  </si>
+  <si>
+    <t>KullanıcıId</t>
+  </si>
+  <si>
+    <t>SağlıkYasamTüyo</t>
+  </si>
+  <si>
+    <t>TüyoID</t>
+  </si>
+  <si>
+    <t>TüyoText</t>
+  </si>
+  <si>
+    <t>Motivasyon</t>
+  </si>
+  <si>
+    <t>YiyecekBilgisiID</t>
+  </si>
+  <si>
+    <t>YiyecekBilgisi</t>
+  </si>
+  <si>
+    <t>YiyecekBilgisiText</t>
+  </si>
+  <si>
+    <t>Bire-Bir İlişki</t>
+  </si>
+  <si>
+    <t>Bire-Çok</t>
+  </si>
+  <si>
+    <t>Çoka-Çok</t>
+  </si>
+  <si>
+    <t>Besin</t>
+  </si>
+  <si>
+    <t>BesinID</t>
+  </si>
+  <si>
+    <t>BesinAd</t>
+  </si>
+  <si>
+    <t>Miktar</t>
+  </si>
+  <si>
+    <t>Notlar</t>
+  </si>
+  <si>
+    <t>OluşturulmaZamanı</t>
+  </si>
+  <si>
+    <t>(DateTime)</t>
   </si>
 </sst>
 </file>
@@ -303,7 +418,7 @@
     <numFmt numFmtId="167" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="168" formatCode="d"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,8 +595,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -572,8 +694,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -719,6 +853,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -750,7 +899,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -997,21 +1146,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="168" fontId="11" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1022,15 +1156,37 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="12" xfId="9" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Ana Başlık" xfId="5" builtinId="15" customBuiltin="1"/>
@@ -1601,8 +1757,8 @@
   <dimension ref="A1:BL40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <pane ySplit="6" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1616,7 +1772,7 @@
     <col min="7" max="7" width="2.6640625" customWidth="1"/>
     <col min="8" max="8" width="6.109375" hidden="1" customWidth="1"/>
     <col min="9" max="18" width="2.5546875" customWidth="1"/>
-    <col min="19" max="19" width="2.5546875" style="93" customWidth="1"/>
+    <col min="19" max="19" width="2.5546875" style="88" customWidth="1"/>
     <col min="20" max="64" width="2.5546875" customWidth="1"/>
     <col min="69" max="70" width="10.33203125"/>
   </cols>
@@ -1655,107 +1811,107 @@
       <c r="B3" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="89"/>
-      <c r="E3" s="97">
+      <c r="D3" s="98"/>
+      <c r="E3" s="102">
         <f ca="1">TODAY()</f>
-        <v>44995</v>
-      </c>
-      <c r="F3" s="98"/>
+        <v>44997</v>
+      </c>
+      <c r="F3" s="103"/>
     </row>
     <row r="4" spans="1:64" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="89"/>
+      <c r="D4" s="98"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="90">
+      <c r="I4" s="99">
         <f ca="1">I5</f>
-        <v>44991</v>
-      </c>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="91"/>
-      <c r="M4" s="91"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="90">
+        <v>44998</v>
+      </c>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
+      <c r="N4" s="100"/>
+      <c r="O4" s="101"/>
+      <c r="P4" s="99">
         <f ca="1">P5</f>
-        <v>44998</v>
-      </c>
-      <c r="Q4" s="91"/>
-      <c r="R4" s="91"/>
-      <c r="S4" s="91"/>
-      <c r="T4" s="91"/>
-      <c r="U4" s="91"/>
-      <c r="V4" s="92"/>
-      <c r="W4" s="90">
+        <v>45005</v>
+      </c>
+      <c r="Q4" s="100"/>
+      <c r="R4" s="100"/>
+      <c r="S4" s="100"/>
+      <c r="T4" s="100"/>
+      <c r="U4" s="100"/>
+      <c r="V4" s="101"/>
+      <c r="W4" s="99">
         <f ca="1">W5</f>
-        <v>45005</v>
-      </c>
-      <c r="X4" s="91"/>
-      <c r="Y4" s="91"/>
-      <c r="Z4" s="91"/>
-      <c r="AA4" s="91"/>
-      <c r="AB4" s="91"/>
-      <c r="AC4" s="92"/>
-      <c r="AD4" s="90">
+        <v>45012</v>
+      </c>
+      <c r="X4" s="100"/>
+      <c r="Y4" s="100"/>
+      <c r="Z4" s="100"/>
+      <c r="AA4" s="100"/>
+      <c r="AB4" s="100"/>
+      <c r="AC4" s="101"/>
+      <c r="AD4" s="99">
         <f ca="1">AD5</f>
-        <v>45012</v>
-      </c>
-      <c r="AE4" s="91"/>
-      <c r="AF4" s="91"/>
-      <c r="AG4" s="91"/>
-      <c r="AH4" s="91"/>
-      <c r="AI4" s="91"/>
-      <c r="AJ4" s="92"/>
-      <c r="AK4" s="90">
+        <v>45019</v>
+      </c>
+      <c r="AE4" s="100"/>
+      <c r="AF4" s="100"/>
+      <c r="AG4" s="100"/>
+      <c r="AH4" s="100"/>
+      <c r="AI4" s="100"/>
+      <c r="AJ4" s="101"/>
+      <c r="AK4" s="99">
         <f ca="1">AK5</f>
-        <v>45019</v>
-      </c>
-      <c r="AL4" s="91"/>
-      <c r="AM4" s="91"/>
-      <c r="AN4" s="91"/>
-      <c r="AO4" s="91"/>
-      <c r="AP4" s="91"/>
-      <c r="AQ4" s="92"/>
-      <c r="AR4" s="90">
+        <v>45026</v>
+      </c>
+      <c r="AL4" s="100"/>
+      <c r="AM4" s="100"/>
+      <c r="AN4" s="100"/>
+      <c r="AO4" s="100"/>
+      <c r="AP4" s="100"/>
+      <c r="AQ4" s="101"/>
+      <c r="AR4" s="99">
         <f ca="1">AR5</f>
-        <v>45026</v>
-      </c>
-      <c r="AS4" s="91"/>
-      <c r="AT4" s="91"/>
-      <c r="AU4" s="91"/>
-      <c r="AV4" s="91"/>
-      <c r="AW4" s="91"/>
-      <c r="AX4" s="92"/>
-      <c r="AY4" s="90">
+        <v>45033</v>
+      </c>
+      <c r="AS4" s="100"/>
+      <c r="AT4" s="100"/>
+      <c r="AU4" s="100"/>
+      <c r="AV4" s="100"/>
+      <c r="AW4" s="100"/>
+      <c r="AX4" s="101"/>
+      <c r="AY4" s="99">
         <f ca="1">AY5</f>
-        <v>45033</v>
-      </c>
-      <c r="AZ4" s="91"/>
-      <c r="BA4" s="91"/>
-      <c r="BB4" s="91"/>
-      <c r="BC4" s="91"/>
-      <c r="BD4" s="91"/>
-      <c r="BE4" s="92"/>
-      <c r="BF4" s="90">
+        <v>45040</v>
+      </c>
+      <c r="AZ4" s="100"/>
+      <c r="BA4" s="100"/>
+      <c r="BB4" s="100"/>
+      <c r="BC4" s="100"/>
+      <c r="BD4" s="100"/>
+      <c r="BE4" s="101"/>
+      <c r="BF4" s="99">
         <f ca="1">BF5</f>
-        <v>45040</v>
-      </c>
-      <c r="BG4" s="91"/>
-      <c r="BH4" s="91"/>
-      <c r="BI4" s="91"/>
-      <c r="BJ4" s="91"/>
-      <c r="BK4" s="91"/>
-      <c r="BL4" s="92"/>
+        <v>45047</v>
+      </c>
+      <c r="BG4" s="100"/>
+      <c r="BH4" s="100"/>
+      <c r="BI4" s="100"/>
+      <c r="BJ4" s="100"/>
+      <c r="BK4" s="100"/>
+      <c r="BL4" s="101"/>
     </row>
     <row r="5" spans="1:64" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="59" t="s">
@@ -1769,227 +1925,227 @@
       <c r="G5" s="84"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>44991</v>
+        <v>44998</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">I5+1</f>
-        <v>44992</v>
+        <v>44999</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>44993</v>
+        <v>45000</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44994</v>
+        <v>45001</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44995</v>
+        <v>45002</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44996</v>
+        <v>45003</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44997</v>
+        <v>45004</v>
       </c>
       <c r="P5" s="11">
         <f ca="1">O5+1</f>
-        <v>44998</v>
+        <v>45005</v>
       </c>
       <c r="Q5" s="10">
         <f ca="1">P5+1</f>
-        <v>44999</v>
+        <v>45006</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45000</v>
-      </c>
-      <c r="S5" s="94">
+        <v>45007</v>
+      </c>
+      <c r="S5" s="89">
         <f t="shared" ca="1" si="0"/>
-        <v>45001</v>
+        <v>45008</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45002</v>
+        <v>45009</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45003</v>
+        <v>45010</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45004</v>
+        <v>45011</v>
       </c>
       <c r="W5" s="11">
         <f ca="1">V5+1</f>
-        <v>45005</v>
+        <v>45012</v>
       </c>
       <c r="X5" s="10">
         <f ca="1">W5+1</f>
-        <v>45006</v>
+        <v>45013</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45007</v>
+        <v>45014</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45008</v>
+        <v>45015</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45009</v>
+        <v>45016</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45010</v>
+        <v>45017</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45011</v>
+        <v>45018</v>
       </c>
       <c r="AD5" s="11">
         <f ca="1">AC5+1</f>
-        <v>45012</v>
+        <v>45019</v>
       </c>
       <c r="AE5" s="10">
         <f ca="1">AD5+1</f>
-        <v>45013</v>
+        <v>45020</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45014</v>
+        <v>45021</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45015</v>
+        <v>45022</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45016</v>
+        <v>45023</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45017</v>
+        <v>45024</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45018</v>
+        <v>45025</v>
       </c>
       <c r="AK5" s="11">
         <f ca="1">AJ5+1</f>
-        <v>45019</v>
+        <v>45026</v>
       </c>
       <c r="AL5" s="10">
         <f ca="1">AK5+1</f>
-        <v>45020</v>
+        <v>45027</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45021</v>
+        <v>45028</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45022</v>
+        <v>45029</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45023</v>
+        <v>45030</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45024</v>
+        <v>45031</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45025</v>
+        <v>45032</v>
       </c>
       <c r="AR5" s="11">
         <f ca="1">AQ5+1</f>
-        <v>45026</v>
+        <v>45033</v>
       </c>
       <c r="AS5" s="10">
         <f ca="1">AR5+1</f>
-        <v>45027</v>
+        <v>45034</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45028</v>
+        <v>45035</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45029</v>
+        <v>45036</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45030</v>
+        <v>45037</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45031</v>
+        <v>45038</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45032</v>
+        <v>45039</v>
       </c>
       <c r="AY5" s="11">
         <f ca="1">AX5+1</f>
-        <v>45033</v>
+        <v>45040</v>
       </c>
       <c r="AZ5" s="10">
         <f ca="1">AY5+1</f>
-        <v>45034</v>
+        <v>45041</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>45035</v>
+        <v>45042</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45036</v>
+        <v>45043</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45037</v>
+        <v>45044</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45038</v>
+        <v>45045</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" ca="1" si="1"/>
-        <v>45039</v>
+        <v>45046</v>
       </c>
       <c r="BF5" s="11">
         <f ca="1">BE5+1</f>
-        <v>45040</v>
+        <v>45047</v>
       </c>
       <c r="BG5" s="10">
         <f ca="1">BF5+1</f>
-        <v>45041</v>
+        <v>45048</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>45042</v>
+        <v>45049</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45043</v>
+        <v>45050</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45044</v>
+        <v>45051</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45045</v>
+        <v>45052</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" ca="1" si="2"/>
-        <v>45046</v>
+        <v>45053</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2055,7 +2211,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
-      <c r="S6" s="95" t="str">
+      <c r="S6" s="90" t="str">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
@@ -2260,7 +2416,7 @@
       <c r="P7" s="44"/>
       <c r="Q7" s="44"/>
       <c r="R7" s="44"/>
-      <c r="S7" s="96"/>
+      <c r="S7" s="91"/>
       <c r="T7" s="44"/>
       <c r="U7" s="44"/>
       <c r="V7" s="44"/>
@@ -2333,7 +2489,7 @@
       <c r="P8" s="44"/>
       <c r="Q8" s="44"/>
       <c r="R8" s="44"/>
-      <c r="S8" s="96"/>
+      <c r="S8" s="91"/>
       <c r="T8" s="44"/>
       <c r="U8" s="44"/>
       <c r="V8" s="44"/>
@@ -2391,15 +2547,15 @@
         <v>66</v>
       </c>
       <c r="D9" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="65">
-        <f ca="1">Project_Start</f>
-        <v>44995</v>
+        <f t="shared" ref="E9:E17" ca="1" si="7">Project_Start</f>
+        <v>44997</v>
       </c>
       <c r="F9" s="65">
-        <f ca="1">E9+1</f>
-        <v>44996</v>
+        <f t="shared" ref="F9:F17" ca="1" si="8">E9+1</f>
+        <v>44998</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17">
@@ -2416,7 +2572,7 @@
       <c r="P9" s="44"/>
       <c r="Q9" s="44"/>
       <c r="R9" s="44"/>
-      <c r="S9" s="96"/>
+      <c r="S9" s="91"/>
       <c r="T9" s="44"/>
       <c r="U9" s="44"/>
       <c r="V9" s="44"/>
@@ -2474,15 +2630,15 @@
         <v>68</v>
       </c>
       <c r="D10" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="65">
-        <f ca="1">Project_Start</f>
-        <v>44995</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>44997</v>
       </c>
       <c r="F10" s="65">
-        <f ca="1">E10+1</f>
-        <v>44996</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>44998</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17">
@@ -2499,7 +2655,7 @@
       <c r="P10" s="44"/>
       <c r="Q10" s="44"/>
       <c r="R10" s="44"/>
-      <c r="S10" s="96"/>
+      <c r="S10" s="91"/>
       <c r="T10" s="44"/>
       <c r="U10" s="45"/>
       <c r="V10" s="45"/>
@@ -2548,22 +2704,22 @@
     </row>
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="58"/>
-      <c r="B11" s="99" t="s">
+      <c r="B11" s="92" t="s">
         <v>58</v>
       </c>
       <c r="C11" s="71" t="s">
         <v>67</v>
       </c>
       <c r="D11" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="65">
-        <f ca="1">Project_Start</f>
-        <v>44995</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>44997</v>
       </c>
       <c r="F11" s="65">
-        <f ca="1">E11+1</f>
-        <v>44996</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>44998</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17">
@@ -2580,7 +2736,7 @@
       <c r="P11" s="44"/>
       <c r="Q11" s="44"/>
       <c r="R11" s="44"/>
-      <c r="S11" s="96"/>
+      <c r="S11" s="91"/>
       <c r="T11" s="44"/>
       <c r="U11" s="44"/>
       <c r="V11" s="44"/>
@@ -2629,22 +2785,22 @@
     </row>
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="58"/>
-      <c r="B12" s="99" t="s">
+      <c r="B12" s="92" t="s">
         <v>59</v>
       </c>
       <c r="C12" s="71" t="s">
         <v>67</v>
       </c>
       <c r="D12" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="65">
-        <f ca="1">Project_Start</f>
-        <v>44995</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>44997</v>
       </c>
       <c r="F12" s="65">
-        <f ca="1">E12+1</f>
-        <v>44996</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>44998</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17">
@@ -2661,7 +2817,7 @@
       <c r="P12" s="44"/>
       <c r="Q12" s="44"/>
       <c r="R12" s="44"/>
-      <c r="S12" s="96"/>
+      <c r="S12" s="91"/>
       <c r="T12" s="44"/>
       <c r="U12" s="44"/>
       <c r="V12" s="44"/>
@@ -2710,20 +2866,22 @@
     </row>
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="58"/>
-      <c r="B13" s="99" t="s">
+      <c r="B13" s="92" t="s">
         <v>60</v>
       </c>
       <c r="C13" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="22"/>
+      <c r="D13" s="22">
+        <v>1</v>
+      </c>
       <c r="E13" s="65">
-        <f ca="1">Project_Start</f>
-        <v>44995</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>44997</v>
       </c>
       <c r="F13" s="65">
-        <f ca="1">E13+1</f>
-        <v>44996</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>44998</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
@@ -2737,7 +2895,7 @@
       <c r="P13" s="44"/>
       <c r="Q13" s="44"/>
       <c r="R13" s="44"/>
-      <c r="S13" s="96"/>
+      <c r="S13" s="91"/>
       <c r="T13" s="44"/>
       <c r="U13" s="44"/>
       <c r="V13" s="44"/>
@@ -2786,20 +2944,22 @@
     </row>
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="58"/>
-      <c r="B14" s="99" t="s">
+      <c r="B14" s="92" t="s">
         <v>61</v>
       </c>
       <c r="C14" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="22"/>
+      <c r="D14" s="22">
+        <v>1</v>
+      </c>
       <c r="E14" s="65">
-        <f ca="1">Project_Start</f>
-        <v>44995</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>44997</v>
       </c>
       <c r="F14" s="65">
-        <f ca="1">E14+1</f>
-        <v>44996</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>44998</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -2813,7 +2973,7 @@
       <c r="P14" s="44"/>
       <c r="Q14" s="44"/>
       <c r="R14" s="44"/>
-      <c r="S14" s="96"/>
+      <c r="S14" s="91"/>
       <c r="T14" s="44"/>
       <c r="U14" s="44"/>
       <c r="V14" s="44"/>
@@ -2868,14 +3028,16 @@
       <c r="C15" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="22"/>
+      <c r="D15" s="22">
+        <v>1</v>
+      </c>
       <c r="E15" s="65">
-        <f ca="1">Project_Start</f>
-        <v>44995</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>44997</v>
       </c>
       <c r="F15" s="65">
-        <f ca="1">E15+1</f>
-        <v>44996</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>44998</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
@@ -2889,7 +3051,7 @@
       <c r="P15" s="44"/>
       <c r="Q15" s="44"/>
       <c r="R15" s="44"/>
-      <c r="S15" s="96"/>
+      <c r="S15" s="91"/>
       <c r="T15" s="44"/>
       <c r="U15" s="44"/>
       <c r="V15" s="44"/>
@@ -2944,14 +3106,16 @@
       <c r="C16" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="22"/>
+      <c r="D16" s="22">
+        <v>1</v>
+      </c>
       <c r="E16" s="65">
-        <f ca="1">Project_Start</f>
-        <v>44995</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>44997</v>
       </c>
       <c r="F16" s="65">
-        <f ca="1">E16+1</f>
-        <v>44996</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>44998</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
@@ -2965,7 +3129,7 @@
       <c r="P16" s="44"/>
       <c r="Q16" s="44"/>
       <c r="R16" s="44"/>
-      <c r="S16" s="96"/>
+      <c r="S16" s="91"/>
       <c r="T16" s="44"/>
       <c r="U16" s="44"/>
       <c r="V16" s="44"/>
@@ -3020,14 +3184,16 @@
       <c r="C17" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="22"/>
+      <c r="D17" s="22">
+        <v>1</v>
+      </c>
       <c r="E17" s="65">
-        <f ca="1">Project_Start</f>
-        <v>44995</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>44997</v>
       </c>
       <c r="F17" s="65">
-        <f ca="1">E17+1</f>
-        <v>44996</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>44998</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
@@ -3041,7 +3207,7 @@
       <c r="P17" s="44"/>
       <c r="Q17" s="44"/>
       <c r="R17" s="44"/>
-      <c r="S17" s="96"/>
+      <c r="S17" s="91"/>
       <c r="T17" s="44"/>
       <c r="U17" s="44"/>
       <c r="V17" s="44"/>
@@ -3114,7 +3280,7 @@
       <c r="P18" s="44"/>
       <c r="Q18" s="44"/>
       <c r="R18" s="44"/>
-      <c r="S18" s="96"/>
+      <c r="S18" s="91"/>
       <c r="T18" s="44"/>
       <c r="U18" s="44"/>
       <c r="V18" s="44"/>
@@ -3168,20 +3334,20 @@
       </c>
       <c r="C19" s="73"/>
       <c r="D19" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="66">
         <f ca="1">F17</f>
-        <v>44996</v>
+        <v>44998</v>
       </c>
       <c r="F19" s="66">
-        <f ca="1">E19+4</f>
-        <v>45000</v>
+        <f ca="1">E19+1</f>
+        <v>44999</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I19" s="44"/>
       <c r="J19" s="44"/>
@@ -3193,7 +3359,7 @@
       <c r="P19" s="44"/>
       <c r="Q19" s="44"/>
       <c r="R19" s="44"/>
-      <c r="S19" s="96"/>
+      <c r="S19" s="91"/>
       <c r="T19" s="44"/>
       <c r="U19" s="44"/>
       <c r="V19" s="44"/>
@@ -3251,11 +3417,11 @@
       </c>
       <c r="E20" s="66">
         <f ca="1">E19+2</f>
-        <v>44998</v>
+        <v>45000</v>
       </c>
       <c r="F20" s="66">
         <f ca="1">E20+5</f>
-        <v>45003</v>
+        <v>45005</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="17">
@@ -3272,7 +3438,7 @@
       <c r="P20" s="44"/>
       <c r="Q20" s="44"/>
       <c r="R20" s="44"/>
-      <c r="S20" s="96"/>
+      <c r="S20" s="91"/>
       <c r="T20" s="44"/>
       <c r="U20" s="45"/>
       <c r="V20" s="45"/>
@@ -3328,11 +3494,11 @@
       <c r="D21" s="27"/>
       <c r="E21" s="66">
         <f ca="1">F20</f>
-        <v>45003</v>
+        <v>45005</v>
       </c>
       <c r="F21" s="66">
         <f ca="1">E21+3</f>
-        <v>45006</v>
+        <v>45008</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17">
@@ -3349,7 +3515,7 @@
       <c r="P21" s="44"/>
       <c r="Q21" s="44"/>
       <c r="R21" s="44"/>
-      <c r="S21" s="96"/>
+      <c r="S21" s="91"/>
       <c r="T21" s="44"/>
       <c r="U21" s="44"/>
       <c r="V21" s="44"/>
@@ -3405,11 +3571,11 @@
       <c r="D22" s="27"/>
       <c r="E22" s="66">
         <f ca="1">E21</f>
-        <v>45003</v>
+        <v>45005</v>
       </c>
       <c r="F22" s="66">
         <f ca="1">E22+2</f>
-        <v>45005</v>
+        <v>45007</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17">
@@ -3426,7 +3592,7 @@
       <c r="P22" s="44"/>
       <c r="Q22" s="44"/>
       <c r="R22" s="44"/>
-      <c r="S22" s="96"/>
+      <c r="S22" s="91"/>
       <c r="T22" s="44"/>
       <c r="U22" s="44"/>
       <c r="V22" s="44"/>
@@ -3482,11 +3648,11 @@
       <c r="D23" s="27"/>
       <c r="E23" s="66">
         <f ca="1">E22</f>
-        <v>45003</v>
+        <v>45005</v>
       </c>
       <c r="F23" s="66">
         <f ca="1">E23+3</f>
-        <v>45006</v>
+        <v>45008</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17">
@@ -3503,7 +3669,7 @@
       <c r="P23" s="44"/>
       <c r="Q23" s="44"/>
       <c r="R23" s="44"/>
-      <c r="S23" s="96"/>
+      <c r="S23" s="91"/>
       <c r="T23" s="44"/>
       <c r="U23" s="44"/>
       <c r="V23" s="44"/>
@@ -3576,7 +3742,7 @@
       <c r="P24" s="44"/>
       <c r="Q24" s="44"/>
       <c r="R24" s="44"/>
-      <c r="S24" s="96"/>
+      <c r="S24" s="91"/>
       <c r="T24" s="44"/>
       <c r="U24" s="44"/>
       <c r="V24" s="44"/>
@@ -3632,11 +3798,11 @@
       <c r="D25" s="32"/>
       <c r="E25" s="67">
         <f ca="1">E9+15</f>
-        <v>45010</v>
+        <v>45012</v>
       </c>
       <c r="F25" s="67">
         <f ca="1">E25+5</f>
-        <v>45015</v>
+        <v>45017</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="17">
@@ -3653,7 +3819,7 @@
       <c r="P25" s="44"/>
       <c r="Q25" s="44"/>
       <c r="R25" s="44"/>
-      <c r="S25" s="96"/>
+      <c r="S25" s="91"/>
       <c r="T25" s="44"/>
       <c r="U25" s="44"/>
       <c r="V25" s="44"/>
@@ -3709,11 +3875,11 @@
       <c r="D26" s="32"/>
       <c r="E26" s="67">
         <f ca="1">F25+1</f>
-        <v>45016</v>
+        <v>45018</v>
       </c>
       <c r="F26" s="67">
         <f ca="1">E26+4</f>
-        <v>45020</v>
+        <v>45022</v>
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="17">
@@ -3730,7 +3896,7 @@
       <c r="P26" s="44"/>
       <c r="Q26" s="44"/>
       <c r="R26" s="44"/>
-      <c r="S26" s="96"/>
+      <c r="S26" s="91"/>
       <c r="T26" s="44"/>
       <c r="U26" s="44"/>
       <c r="V26" s="44"/>
@@ -3786,11 +3952,11 @@
       <c r="D27" s="32"/>
       <c r="E27" s="67">
         <f ca="1">E26+5</f>
-        <v>45021</v>
+        <v>45023</v>
       </c>
       <c r="F27" s="67">
         <f ca="1">E27+5</f>
-        <v>45026</v>
+        <v>45028</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="17">
@@ -3807,7 +3973,7 @@
       <c r="P27" s="44"/>
       <c r="Q27" s="44"/>
       <c r="R27" s="44"/>
-      <c r="S27" s="96"/>
+      <c r="S27" s="91"/>
       <c r="T27" s="44"/>
       <c r="U27" s="44"/>
       <c r="V27" s="44"/>
@@ -3863,11 +4029,11 @@
       <c r="D28" s="32"/>
       <c r="E28" s="67">
         <f ca="1">F27+1</f>
-        <v>45027</v>
+        <v>45029</v>
       </c>
       <c r="F28" s="67">
         <f ca="1">E28+4</f>
-        <v>45031</v>
+        <v>45033</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="17">
@@ -3884,7 +4050,7 @@
       <c r="P28" s="44"/>
       <c r="Q28" s="44"/>
       <c r="R28" s="44"/>
-      <c r="S28" s="96"/>
+      <c r="S28" s="91"/>
       <c r="T28" s="44"/>
       <c r="U28" s="44"/>
       <c r="V28" s="44"/>
@@ -3940,11 +4106,11 @@
       <c r="D29" s="32"/>
       <c r="E29" s="67">
         <f ca="1">E27</f>
-        <v>45021</v>
+        <v>45023</v>
       </c>
       <c r="F29" s="67">
         <f ca="1">E29+4</f>
-        <v>45025</v>
+        <v>45027</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="17">
@@ -3961,7 +4127,7 @@
       <c r="P29" s="44"/>
       <c r="Q29" s="44"/>
       <c r="R29" s="44"/>
-      <c r="S29" s="96"/>
+      <c r="S29" s="91"/>
       <c r="T29" s="44"/>
       <c r="U29" s="44"/>
       <c r="V29" s="44"/>
@@ -4034,7 +4200,7 @@
       <c r="P30" s="44"/>
       <c r="Q30" s="44"/>
       <c r="R30" s="44"/>
-      <c r="S30" s="96"/>
+      <c r="S30" s="91"/>
       <c r="T30" s="44"/>
       <c r="U30" s="44"/>
       <c r="V30" s="44"/>
@@ -4109,7 +4275,7 @@
       <c r="P31" s="44"/>
       <c r="Q31" s="44"/>
       <c r="R31" s="44"/>
-      <c r="S31" s="96"/>
+      <c r="S31" s="91"/>
       <c r="T31" s="44"/>
       <c r="U31" s="44"/>
       <c r="V31" s="44"/>
@@ -4184,7 +4350,7 @@
       <c r="P32" s="44"/>
       <c r="Q32" s="44"/>
       <c r="R32" s="44"/>
-      <c r="S32" s="96"/>
+      <c r="S32" s="91"/>
       <c r="T32" s="44"/>
       <c r="U32" s="44"/>
       <c r="V32" s="44"/>
@@ -4259,7 +4425,7 @@
       <c r="P33" s="44"/>
       <c r="Q33" s="44"/>
       <c r="R33" s="44"/>
-      <c r="S33" s="96"/>
+      <c r="S33" s="91"/>
       <c r="T33" s="44"/>
       <c r="U33" s="44"/>
       <c r="V33" s="44"/>
@@ -4334,7 +4500,7 @@
       <c r="P34" s="44"/>
       <c r="Q34" s="44"/>
       <c r="R34" s="44"/>
-      <c r="S34" s="96"/>
+      <c r="S34" s="91"/>
       <c r="T34" s="44"/>
       <c r="U34" s="44"/>
       <c r="V34" s="44"/>
@@ -4409,7 +4575,7 @@
       <c r="P35" s="44"/>
       <c r="Q35" s="44"/>
       <c r="R35" s="44"/>
-      <c r="S35" s="96"/>
+      <c r="S35" s="91"/>
       <c r="T35" s="44"/>
       <c r="U35" s="44"/>
       <c r="V35" s="44"/>
@@ -4480,7 +4646,7 @@
       <c r="P36" s="44"/>
       <c r="Q36" s="44"/>
       <c r="R36" s="44"/>
-      <c r="S36" s="96"/>
+      <c r="S36" s="91"/>
       <c r="T36" s="44"/>
       <c r="U36" s="44"/>
       <c r="V36" s="44"/>
@@ -4553,7 +4719,7 @@
       <c r="P37" s="46"/>
       <c r="Q37" s="46"/>
       <c r="R37" s="46"/>
-      <c r="S37" s="96"/>
+      <c r="S37" s="91"/>
       <c r="T37" s="46"/>
       <c r="U37" s="46"/>
       <c r="V37" s="46"/>
@@ -4694,6 +4860,272 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A04530-A1B5-44C2-B8EE-AAD648FB4777}">
+  <dimension ref="B2:L27"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C4" s="93" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="95" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="104"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="106"/>
+      <c r="K4" s="93" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C5" s="96" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="95"/>
+      <c r="F5" s="94" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="105"/>
+      <c r="I5" s="94" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="94" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C6" s="94" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="94" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="105"/>
+      <c r="I6" s="94" t="s">
+        <v>86</v>
+      </c>
+      <c r="K6" s="94" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C7" s="94" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="95" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="94" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="105"/>
+      <c r="J7" s="95" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" s="94" t="s">
+        <v>104</v>
+      </c>
+      <c r="L7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C8" s="94" t="s">
+        <v>75</v>
+      </c>
+      <c r="K8" s="94" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C9" s="94" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C10" s="94" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C11" s="94" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="93" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="104"/>
+      <c r="I11" s="93" t="s">
+        <v>94</v>
+      </c>
+      <c r="K11" s="93" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C12" s="94" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="94" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="105"/>
+      <c r="I12" s="94" t="s">
+        <v>92</v>
+      </c>
+      <c r="K12" s="94" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C13" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="94" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="105"/>
+      <c r="I13" s="94" t="s">
+        <v>93</v>
+      </c>
+      <c r="K13" s="94" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C14" s="94" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="105"/>
+      <c r="G14" s="105"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="95" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="94" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C16" s="94" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E23" s="94" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="93" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="104"/>
+      <c r="H23" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" s="93" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="H24" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="I24" s="93" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I25" s="93" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I26" s="93" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="H27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I27" s="93" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>

</xml_diff>

<commit_message>
Olusturulan yapıya dair sorularım eklendi
</commit_message>
<xml_diff>
--- a/ProjePlanı.xlsx
+++ b/ProjePlanı.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B8C671-C4EB-4806-97FD-B3715FB0BD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86E28E7-DD67-4C3A-ABC1-BDC33E062B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="855" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="111">
   <si>
     <t>Task 3</t>
   </si>
@@ -405,6 +405,15 @@
   </si>
   <si>
     <t>(DateTime)</t>
+  </si>
+  <si>
+    <t>Sorularım-Berna</t>
+  </si>
+  <si>
+    <t>Yiyecek bilgisi ile besin arasında bir ilişki olmalı mı?</t>
+  </si>
+  <si>
+    <t>Oluşturulma Zamanı Öğünde mi olmalı?</t>
   </si>
 </sst>
 </file>
@@ -1163,30 +1172,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="12" xfId="9" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="12" xfId="9" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Ana Başlık" xfId="5" builtinId="15" customBuiltin="1"/>
@@ -1756,7 +1765,7 @@
   </sheetPr>
   <dimension ref="A1:BL40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" showRuler="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
@@ -1811,13 +1820,13 @@
       <c r="B3" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="97" t="s">
+      <c r="C3" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="98"/>
+      <c r="D3" s="105"/>
       <c r="E3" s="102">
         <f ca="1">TODAY()</f>
-        <v>44997</v>
+        <v>44998</v>
       </c>
       <c r="F3" s="103"/>
     </row>
@@ -1825,10 +1834,10 @@
       <c r="A4" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="98"/>
+      <c r="D4" s="105"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
@@ -2551,11 +2560,11 @@
       </c>
       <c r="E9" s="65">
         <f t="shared" ref="E9:E17" ca="1" si="7">Project_Start</f>
-        <v>44997</v>
+        <v>44998</v>
       </c>
       <c r="F9" s="65">
         <f t="shared" ref="F9:F17" ca="1" si="8">E9+1</f>
-        <v>44998</v>
+        <v>44999</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17">
@@ -2634,11 +2643,11 @@
       </c>
       <c r="E10" s="65">
         <f t="shared" ca="1" si="7"/>
-        <v>44997</v>
+        <v>44998</v>
       </c>
       <c r="F10" s="65">
         <f t="shared" ca="1" si="8"/>
-        <v>44998</v>
+        <v>44999</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17">
@@ -2715,11 +2724,11 @@
       </c>
       <c r="E11" s="65">
         <f t="shared" ca="1" si="7"/>
-        <v>44997</v>
+        <v>44998</v>
       </c>
       <c r="F11" s="65">
         <f t="shared" ca="1" si="8"/>
-        <v>44998</v>
+        <v>44999</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17">
@@ -2796,11 +2805,11 @@
       </c>
       <c r="E12" s="65">
         <f t="shared" ca="1" si="7"/>
-        <v>44997</v>
+        <v>44998</v>
       </c>
       <c r="F12" s="65">
         <f t="shared" ca="1" si="8"/>
-        <v>44998</v>
+        <v>44999</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17">
@@ -2877,11 +2886,11 @@
       </c>
       <c r="E13" s="65">
         <f t="shared" ca="1" si="7"/>
-        <v>44997</v>
+        <v>44998</v>
       </c>
       <c r="F13" s="65">
         <f t="shared" ca="1" si="8"/>
-        <v>44998</v>
+        <v>44999</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
@@ -2955,11 +2964,11 @@
       </c>
       <c r="E14" s="65">
         <f t="shared" ca="1" si="7"/>
-        <v>44997</v>
+        <v>44998</v>
       </c>
       <c r="F14" s="65">
         <f t="shared" ca="1" si="8"/>
-        <v>44998</v>
+        <v>44999</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -3033,11 +3042,11 @@
       </c>
       <c r="E15" s="65">
         <f t="shared" ca="1" si="7"/>
-        <v>44997</v>
+        <v>44998</v>
       </c>
       <c r="F15" s="65">
         <f t="shared" ca="1" si="8"/>
-        <v>44998</v>
+        <v>44999</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
@@ -3111,11 +3120,11 @@
       </c>
       <c r="E16" s="65">
         <f t="shared" ca="1" si="7"/>
-        <v>44997</v>
+        <v>44998</v>
       </c>
       <c r="F16" s="65">
         <f t="shared" ca="1" si="8"/>
-        <v>44998</v>
+        <v>44999</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
@@ -3189,11 +3198,11 @@
       </c>
       <c r="E17" s="65">
         <f t="shared" ca="1" si="7"/>
-        <v>44997</v>
+        <v>44998</v>
       </c>
       <c r="F17" s="65">
         <f t="shared" ca="1" si="8"/>
-        <v>44998</v>
+        <v>44999</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
@@ -3338,11 +3347,11 @@
       </c>
       <c r="E19" s="66">
         <f ca="1">F17</f>
-        <v>44998</v>
+        <v>44999</v>
       </c>
       <c r="F19" s="66">
         <f ca="1">E19+1</f>
-        <v>44999</v>
+        <v>45000</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17">
@@ -3417,11 +3426,11 @@
       </c>
       <c r="E20" s="66">
         <f ca="1">E19+2</f>
-        <v>45000</v>
+        <v>45001</v>
       </c>
       <c r="F20" s="66">
         <f ca="1">E20+5</f>
-        <v>45005</v>
+        <v>45006</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="17">
@@ -3494,11 +3503,11 @@
       <c r="D21" s="27"/>
       <c r="E21" s="66">
         <f ca="1">F20</f>
-        <v>45005</v>
+        <v>45006</v>
       </c>
       <c r="F21" s="66">
         <f ca="1">E21+3</f>
-        <v>45008</v>
+        <v>45009</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17">
@@ -3571,11 +3580,11 @@
       <c r="D22" s="27"/>
       <c r="E22" s="66">
         <f ca="1">E21</f>
-        <v>45005</v>
+        <v>45006</v>
       </c>
       <c r="F22" s="66">
         <f ca="1">E22+2</f>
-        <v>45007</v>
+        <v>45008</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17">
@@ -3648,11 +3657,11 @@
       <c r="D23" s="27"/>
       <c r="E23" s="66">
         <f ca="1">E22</f>
-        <v>45005</v>
+        <v>45006</v>
       </c>
       <c r="F23" s="66">
         <f ca="1">E23+3</f>
-        <v>45008</v>
+        <v>45009</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17">
@@ -3798,11 +3807,11 @@
       <c r="D25" s="32"/>
       <c r="E25" s="67">
         <f ca="1">E9+15</f>
-        <v>45012</v>
+        <v>45013</v>
       </c>
       <c r="F25" s="67">
         <f ca="1">E25+5</f>
-        <v>45017</v>
+        <v>45018</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="17">
@@ -3875,11 +3884,11 @@
       <c r="D26" s="32"/>
       <c r="E26" s="67">
         <f ca="1">F25+1</f>
-        <v>45018</v>
+        <v>45019</v>
       </c>
       <c r="F26" s="67">
         <f ca="1">E26+4</f>
-        <v>45022</v>
+        <v>45023</v>
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="17">
@@ -3952,11 +3961,11 @@
       <c r="D27" s="32"/>
       <c r="E27" s="67">
         <f ca="1">E26+5</f>
-        <v>45023</v>
+        <v>45024</v>
       </c>
       <c r="F27" s="67">
         <f ca="1">E27+5</f>
-        <v>45028</v>
+        <v>45029</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="17">
@@ -4029,11 +4038,11 @@
       <c r="D28" s="32"/>
       <c r="E28" s="67">
         <f ca="1">F27+1</f>
-        <v>45029</v>
+        <v>45030</v>
       </c>
       <c r="F28" s="67">
         <f ca="1">E28+4</f>
-        <v>45033</v>
+        <v>45034</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="17">
@@ -4106,11 +4115,11 @@
       <c r="D29" s="32"/>
       <c r="E29" s="67">
         <f ca="1">E27</f>
-        <v>45023</v>
+        <v>45024</v>
       </c>
       <c r="F29" s="67">
         <f ca="1">E29+4</f>
-        <v>45027</v>
+        <v>45028</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="17">
@@ -4778,17 +4787,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D37">
     <cfRule type="dataBar" priority="14">
@@ -4863,8 +4872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A04530-A1B5-44C2-B8EE-AAD648FB4777}">
   <dimension ref="B2:L27"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4908,12 +4917,12 @@
       <c r="F4" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="G4" s="104"/>
-      <c r="H4" s="106"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="98"/>
       <c r="I4" s="93" t="s">
         <v>86</v>
       </c>
-      <c r="J4" s="106"/>
+      <c r="J4" s="98"/>
       <c r="K4" s="93" t="s">
         <v>101</v>
       </c>
@@ -4926,7 +4935,6 @@
       <c r="F5" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="105"/>
       <c r="I5" s="94" t="s">
         <v>87</v>
       </c>
@@ -4941,7 +4949,6 @@
       <c r="F6" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="105"/>
       <c r="I6" s="94" t="s">
         <v>86</v>
       </c>
@@ -4959,7 +4966,6 @@
       <c r="F7" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="G7" s="105"/>
       <c r="J7" s="95" t="s">
         <v>82</v>
       </c>
@@ -5004,7 +5010,7 @@
       <c r="F11" s="93" t="s">
         <v>91</v>
       </c>
-      <c r="G11" s="104"/>
+      <c r="G11" s="97"/>
       <c r="I11" s="93" t="s">
         <v>94</v>
       </c>
@@ -5019,7 +5025,6 @@
       <c r="F12" s="94" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="105"/>
       <c r="I12" s="94" t="s">
         <v>92</v>
       </c>
@@ -5034,7 +5039,6 @@
       <c r="F13" s="94" t="s">
         <v>93</v>
       </c>
-      <c r="G13" s="105"/>
       <c r="I13" s="94" t="s">
         <v>93</v>
       </c>
@@ -5046,8 +5050,6 @@
       <c r="C14" s="94" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="105"/>
-      <c r="G14" s="105"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="95" t="s">
@@ -5062,7 +5064,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="K21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>98</v>
       </c>
@@ -5072,23 +5079,29 @@
       <c r="H22" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="K22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
       <c r="E23" s="94" t="s">
         <v>86</v>
       </c>
       <c r="F23" s="93" t="s">
         <v>101</v>
       </c>
-      <c r="G23" s="104"/>
+      <c r="G23" s="97"/>
       <c r="H23" t="s">
         <v>71</v>
       </c>
       <c r="I23" s="93" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="K23" s="106" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
       <c r="H24" s="93" t="s">
         <v>83</v>
       </c>
@@ -5096,7 +5109,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
       <c r="H25" t="s">
         <v>71</v>
       </c>
@@ -5104,7 +5117,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
       <c r="H26" t="s">
         <v>71</v>
       </c>
@@ -5112,7 +5125,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
       <c r="H27" t="s">
         <v>71</v>
       </c>

</xml_diff>